<commit_message>
Sum of all allthread working & printing
</commit_message>
<xml_diff>
--- a/DewaltHangerCalculator/LEVEL 2 AREA A HANGERS.xlsx
+++ b/DewaltHangerCalculator/LEVEL 2 AREA A HANGERS.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsahli\source\repos\DewaltHangerCalculator\DewaltHangerCalculator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AF165D-4E6F-47F4-8273-63001AC01D9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="32400" yWindow="45" windowWidth="21210" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13485" windowWidth="21060" xWindow="30750" yWindow="1950"/>
   </bookViews>
   <sheets>
-    <sheet name="LEVEL 2 AREA A HANGERS" sheetId="1" r:id="rId1"/>
+    <sheet name="LEVEL 2 AREA A HANGERS" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Total Strut" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Total Allthread Cuts" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Total Assemblies" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Print Me" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>LEVEL 2 AREA A HANGERS</t>
   </si>
@@ -173,24 +171,121 @@
   </si>
   <si>
     <t>Grand total: 51</t>
+  </si>
+  <si>
+    <t>Total Strut</t>
+  </si>
+  <si>
+    <t>Strut Type</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>BACK TO BACK SHALLOW: 14"</t>
+  </si>
+  <si>
+    <t>BACK TO BACK SHALLOW: 22"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 12 1/2"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 12"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 13"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 14"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 20"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 22"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 6"</t>
+  </si>
+  <si>
+    <t>Total Allthread</t>
+  </si>
+  <si>
+    <t>Allthread Length</t>
+  </si>
+  <si>
+    <t>Total allthread length = 2453.0</t>
+  </si>
+  <si>
+    <t>Assembly Name and Quantity</t>
+  </si>
+  <si>
+    <t>Assembly Name</t>
+  </si>
+  <si>
+    <t>PRINT_ME</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CR-01                                                           TOU: 9' - 4 9/16"                                                                    DEEP STRUT: 6"                                                               Allthread Length: 22"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CR-02                                                           TOU: 9' - 4 9/16"                                                                    DEEP STRUT: 12"                                                               Allthread Length: 22"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-03                                                           TOU: 9' - 3 1/2"                                                                    DEEP STRUT: 12 1/2"                                                               Allthread Length: 23"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-04                                                           TOU: 9' - 3 1/2"                                                                    DEEP STRUT: 13"                                                               Allthread Length: 23"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CR-05                                                           TOU: 9' - 4 9/16"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 22"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-06                                                           TOU: 9' - 3 1/2"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 23"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-07                                                           TOU: 9' - 1 1/2"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 25"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-08                                                           TOU: 8' - 11 1/2"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 27"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-09                                                           TOU: 8' - 10"                                                                    BACK TO BACK SHALLOW: 14"                                                               Allthread Length: 28 1/2"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-10                                                           TOU: 7' - 8"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 42 1/2"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-11                                                           TOU: 10' - 6 1/2"                                                                    DEEP STRUT: 20"                                                               Allthread Length: 8"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-12                                                           TOU: 9' - 9"                                                                    DEEP STRUT: 20"                                                               Allthread Length: 17 1/2"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-13                                                           TOU: 7' - 8"                                                                    DEEP STRUT: 22"                                                               Allthread Length: 42 1/2"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-13                                                           TOU: 7' - 8"                                                                    BACK TO BACK SHALLOW: 22"                                                               Allthread Length: 42 1/2"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -206,26 +301,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -525,29 +614,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33" style="2" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="2" width="26.85546875"/>
+    <col customWidth="1" max="2" min="2" style="2" width="17.28515625"/>
+    <col customWidth="1" max="3" min="3" style="2" width="18.42578125"/>
+    <col customWidth="1" max="4" min="4" style="2" width="31.85546875"/>
+    <col customWidth="1" max="5" min="5" style="2" width="14.42578125"/>
+    <col customWidth="1" max="6" min="6" style="2" width="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -573,7 +666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -599,7 +692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -625,7 +718,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -651,7 +744,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -677,7 +770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -703,7 +796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -729,7 +822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -755,7 +848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -781,7 +874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -807,7 +900,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -833,7 +926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -859,7 +952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -885,7 +978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -911,7 +1004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -937,7 +1030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -963,7 +1056,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -989,7 +1082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1015,7 +1108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1041,7 +1134,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1067,7 +1160,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1093,7 +1186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1119,7 +1212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1264,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1197,7 +1290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1223,7 +1316,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1249,7 +1342,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1275,7 +1368,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1301,7 +1394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1327,7 +1420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1353,7 +1446,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1379,7 +1472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1405,7 +1498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1431,7 +1524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1457,7 +1550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1483,7 +1576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1509,7 +1602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1535,7 +1628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1561,7 +1654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1680,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1639,7 +1732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1665,7 +1758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -1691,7 +1784,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1717,7 +1810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1743,7 +1836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1769,7 +1862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1795,7 +1888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1821,7 +1914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -1847,7 +1940,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -1873,7 +1966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -1899,15 +1992,644 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>50</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55" s="1" t="n">
         <v>1226.5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Allthread length now prints in feet instead of inches
</commit_message>
<xml_diff>
--- a/DewaltHangerCalculator/LEVEL 2 AREA A HANGERS.xlsx
+++ b/DewaltHangerCalculator/LEVEL 2 AREA A HANGERS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13485" windowWidth="21060" xWindow="30750" yWindow="1950"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13485" windowWidth="21060" xWindow="31665" yWindow="405"/>
   </bookViews>
   <sheets>
     <sheet name="LEVEL 2 AREA A HANGERS" sheetId="1" state="visible" r:id="rId1"/>
@@ -215,7 +215,7 @@
     <t>Allthread Length</t>
   </si>
   <si>
-    <t>Total allthread length = 2453.0</t>
+    <t>Total allthread length = 2453.0 ft</t>
   </si>
   <si>
     <t>Assembly Name and Quantity</t>
@@ -621,7 +621,7 @@
   </sheetPr>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Last line is now counted. Total strut is now summed in feet, but not by category.
</commit_message>
<xml_diff>
--- a/DewaltHangerCalculator/LEVEL 2 AREA A HANGERS.xlsx
+++ b/DewaltHangerCalculator/LEVEL 2 AREA A HANGERS.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsahli\source\repos\DewaltHangerCalculator\DewaltHangerCalculator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A30473-A60F-47E5-88DB-8219C84F8AB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16440" windowWidth="29040" xWindow="28680" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="LEVEL 2 AREA A HANGERS" sheetId="1" r:id="rId1"/>
+    <sheet name="LEVEL 2 AREA A HANGERS" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Total Strut" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Total Allthread Cuts" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Total Assemblies" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Print Me" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>LEVEL 2 AREA A HANGERS</t>
   </si>
@@ -172,25 +170,122 @@
     <t>DEWALT RT-02</t>
   </si>
   <si>
-    <t>Grand total: 51</t>
+    <t>Total Strut</t>
+  </si>
+  <si>
+    <t>Strut Type</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>BACK TO BACK SHALLOW: 14"</t>
+  </si>
+  <si>
+    <t>BACK TO BACK SHALLOW: 22"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 12 1/2"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 12"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 13"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 14"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 20"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 22"</t>
+  </si>
+  <si>
+    <t>DEEP STRUT: 6"</t>
+  </si>
+  <si>
+    <t>Total strut length = 59.375 ft</t>
+  </si>
+  <si>
+    <t>Total Allthread</t>
+  </si>
+  <si>
+    <t>Allthread Length</t>
+  </si>
+  <si>
+    <t>Total allthread length = 204.416666667 ft</t>
+  </si>
+  <si>
+    <t>Assembly Name and Quantity</t>
+  </si>
+  <si>
+    <t>Assembly Name</t>
+  </si>
+  <si>
+    <t>PRINT_ME</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CR-01                                                           TOU: 9' - 4 9/16"                                                                    DEEP STRUT: 6"                                                               Allthread Length: 22"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CR-02                                                           TOU: 9' - 4 9/16"                                                                    DEEP STRUT: 12"                                                               Allthread Length: 22"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-03                                                           TOU: 9' - 3 1/2"                                                                    DEEP STRUT: 12 1/2"                                                               Allthread Length: 23"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-04                                                           TOU: 9' - 3 1/2"                                                                    DEEP STRUT: 13"                                                               Allthread Length: 23"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CR-05                                                           TOU: 9' - 4 9/16"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 22"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-06                                                           TOU: 9' - 3 1/2"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 23"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-07                                                           TOU: 9' - 1 1/2"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 25"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-08                                                           TOU: 8' - 11 1/2"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 27"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-09                                                           TOU: 8' - 10"                                                                    BACK TO BACK SHALLOW: 14"                                                               Allthread Length: 28 1/2"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-10                                                           TOU: 7' - 8"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 42 1/2"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-11                                                           TOU: 10' - 6 1/2"                                                                    DEEP STRUT: 20"                                                               Allthread Length: 8"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-12                                                           TOU: 9' - 9"                                                                    DEEP STRUT: 20"                                                               Allthread Length: 17 1/2"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-13                                                           TOU: 7' - 8"                                                                    DEEP STRUT: 22"                                                               Allthread Length: 42 1/2"</t>
+  </si>
+  <si>
+    <t>LEVEL 2 AREA A Tag: CT-13                                                           TOU: 7' - 8"                                                                    BACK TO BACK SHALLOW: 22"                                                               Allthread Length: 42 1/2"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -206,26 +301,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -525,29 +613,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33" style="2" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="26.85546875"/>
+    <col customWidth="1" max="2" min="2" style="1" width="17.28515625"/>
+    <col customWidth="1" max="3" min="3" style="1" width="18.42578125"/>
+    <col customWidth="1" max="4" min="4" style="1" width="31.85546875"/>
+    <col customWidth="1" max="5" min="5" style="1" width="14.42578125"/>
+    <col customWidth="1" max="6" min="6" style="1" width="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -573,7 +665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -599,7 +691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -625,7 +717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -651,7 +743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -677,7 +769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -703,7 +795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -729,7 +821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -755,7 +847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -781,7 +873,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -807,7 +899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -833,7 +925,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -859,7 +951,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -885,7 +977,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -911,7 +1003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -937,7 +1029,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -963,7 +1055,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -989,7 +1081,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1015,7 +1107,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1041,7 +1133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1067,7 +1159,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1093,7 +1185,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1119,7 +1211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1263,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1197,7 +1289,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1223,7 +1315,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1249,7 +1341,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1275,7 +1367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1301,7 +1393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1327,7 +1419,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1353,7 +1445,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1379,7 +1471,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1405,7 +1497,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1431,7 +1523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1457,7 +1549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1483,7 +1575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1509,7 +1601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1535,7 +1627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1561,7 +1653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1639,7 +1731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1665,7 +1757,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -1691,7 +1783,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1717,7 +1809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1743,7 +1835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1769,7 +1861,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1795,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1821,7 +1913,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -1847,67 +1939,696 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="53" spans="1:8"/>
+    <row r="54" spans="1:8"/>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
         <v>48</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>39</v>
       </c>
-      <c r="D53" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" t="s">
         <v>14</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F55" t="s">
         <v>40</v>
       </c>
-      <c r="G53" t="s">
-        <v>15</v>
-      </c>
-      <c r="H53" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>9</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="G55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8"/>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" t="s">
         <v>48</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C57" t="s">
         <v>39</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D57" t="s">
         <v>36</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E57" t="s">
         <v>14</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F57" t="s">
         <v>40</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G57" t="s">
         <v>49</v>
       </c>
-      <c r="H54" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="H57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F55" s="1">
-        <v>1226.5</v>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sum of strut and allthread are rounded to 2 decimal points
</commit_message>
<xml_diff>
--- a/DewaltHangerCalculator/LEVEL 2 AREA A HANGERS.xlsx
+++ b/DewaltHangerCalculator/LEVEL 2 AREA A HANGERS.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsahli\source\repos\DewaltHangerCalculator\DewaltHangerCalculator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92FD731-62CD-4936-948A-BF3359D058C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16440" windowWidth="29040" xWindow="28680" yWindow="-120"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LEVEL 2 AREA A HANGERS" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Total Strut" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Total Allthread Cuts" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Total Assemblies" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Print Me" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="LEVEL 2 AREA A HANGERS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="50">
   <si>
     <t>LEVEL 2 AREA A HANGERS</t>
   </si>
@@ -168,124 +170,24 @@
   </si>
   <si>
     <t>DEWALT RT-02</t>
-  </si>
-  <si>
-    <t>Total Strut</t>
-  </si>
-  <si>
-    <t>Strut Type</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>BACK TO BACK SHALLOW: 14"</t>
-  </si>
-  <si>
-    <t>BACK TO BACK SHALLOW: 22"</t>
-  </si>
-  <si>
-    <t>DEEP STRUT: 12 1/2"</t>
-  </si>
-  <si>
-    <t>DEEP STRUT: 12"</t>
-  </si>
-  <si>
-    <t>DEEP STRUT: 13"</t>
-  </si>
-  <si>
-    <t>DEEP STRUT: 14"</t>
-  </si>
-  <si>
-    <t>DEEP STRUT: 20"</t>
-  </si>
-  <si>
-    <t>DEEP STRUT: 22"</t>
-  </si>
-  <si>
-    <t>DEEP STRUT: 6"</t>
-  </si>
-  <si>
-    <t>Total strut length = 59.375 ft</t>
-  </si>
-  <si>
-    <t>Total Allthread</t>
-  </si>
-  <si>
-    <t>Allthread Length</t>
-  </si>
-  <si>
-    <t>Total allthread length = 204.416666667 ft</t>
-  </si>
-  <si>
-    <t>Assembly Name and Quantity</t>
-  </si>
-  <si>
-    <t>Assembly Name</t>
-  </si>
-  <si>
-    <t>PRINT_ME</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CR-01                                                           TOU: 9' - 4 9/16"                                                                    DEEP STRUT: 6"                                                               Allthread Length: 22"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CR-02                                                           TOU: 9' - 4 9/16"                                                                    DEEP STRUT: 12"                                                               Allthread Length: 22"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-03                                                           TOU: 9' - 3 1/2"                                                                    DEEP STRUT: 12 1/2"                                                               Allthread Length: 23"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-04                                                           TOU: 9' - 3 1/2"                                                                    DEEP STRUT: 13"                                                               Allthread Length: 23"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CR-05                                                           TOU: 9' - 4 9/16"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 22"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-06                                                           TOU: 9' - 3 1/2"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 23"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-07                                                           TOU: 9' - 1 1/2"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 25"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-08                                                           TOU: 8' - 11 1/2"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 27"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-09                                                           TOU: 8' - 10"                                                                    BACK TO BACK SHALLOW: 14"                                                               Allthread Length: 28 1/2"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-10                                                           TOU: 7' - 8"                                                                    DEEP STRUT: 14"                                                               Allthread Length: 42 1/2"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-11                                                           TOU: 10' - 6 1/2"                                                                    DEEP STRUT: 20"                                                               Allthread Length: 8"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-12                                                           TOU: 9' - 9"                                                                    DEEP STRUT: 20"                                                               Allthread Length: 17 1/2"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-13                                                           TOU: 7' - 8"                                                                    DEEP STRUT: 22"                                                               Allthread Length: 42 1/2"</t>
-  </si>
-  <si>
-    <t>LEVEL 2 AREA A Tag: CT-13                                                           TOU: 7' - 8"                                                                    BACK TO BACK SHALLOW: 22"                                                               Allthread Length: 42 1/2"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -301,19 +203,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -613,33 +521,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="26.85546875"/>
-    <col customWidth="1" max="2" min="2" style="1" width="17.28515625"/>
-    <col customWidth="1" max="3" min="3" style="1" width="18.42578125"/>
-    <col customWidth="1" max="4" min="4" style="1" width="31.85546875"/>
-    <col customWidth="1" max="5" min="5" style="1" width="14.42578125"/>
-    <col customWidth="1" max="6" min="6" style="1" width="33"/>
+    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -665,7 +569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -691,7 +595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -717,7 +621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -743,7 +647,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -769,7 +673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -795,7 +699,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -821,7 +725,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -847,7 +751,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -873,7 +777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -899,7 +803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -925,7 +829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -951,7 +855,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -977,7 +881,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1003,7 +907,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1029,7 +933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1055,7 +959,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +985,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1107,7 +1011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1133,7 +1037,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1159,7 +1063,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1211,7 +1115,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1167,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1289,7 +1193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1315,7 +1219,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1341,7 +1245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1367,7 +1271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1393,7 +1297,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1419,7 +1323,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1445,7 +1349,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1471,7 +1375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1497,7 +1401,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1523,7 +1427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1549,7 +1453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1575,7 +1479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1601,7 +1505,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1627,7 +1531,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1653,7 +1557,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1679,7 +1583,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1705,7 +1609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1731,7 +1635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1757,7 +1661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -1783,7 +1687,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1809,7 +1713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1835,7 +1739,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1861,7 +1765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1887,7 +1791,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1913,7 +1817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -1939,9 +1843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:8"/>
-    <row r="54" spans="1:8"/>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -1967,8 +1869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:8"/>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -1995,640 +1896,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B2"/>
-  </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B2"/>
-  </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B2"/>
-  </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>